<commit_message>
v2.0.0 (spreadsheet version) (Feb 2023)
Japanese translation of description in MASVS-NETWORK v2.0.0
</commit_message>
<xml_diff>
--- a/Document-2.0.0-ja-xlsx/MASVS v2.0.0-ja.xlsx
+++ b/Document-2.0.0-ja-xlsx/MASVS v2.0.0-ja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\docs\owasp-masvs\owasp-masvs-ja-master\Document-2.0.0-ja-xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E364E6BB-F678-47DB-839B-D7438628EAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DACB3-B77E-4AC1-8755-69BF6038611D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>MASVS-STORAGE-2</t>
-  </si>
-  <si>
-    <t>There are cases when sensitive data is unintentionally stored or exposed to publicly accessible locations; typically as a side-effect of using certain APIs, system capabilities such as backups or logs. This control covers this kind of unintentional leaks where the developer actually has a way to prevent it.</t>
   </si>
   <si>
     <t>MSTG-STORAGE-3, MSTG-STORAGE-4, MSTG-STORAGE-5, MSTG-STORAGE-8</t>
@@ -1138,7 +1135,168 @@
     <phoneticPr fontId="32"/>
   </si>
   <si>
-    <t>Apps handle sensitive data coming from many sources such as the user, the backend, system services or other apps on the device and usually need to store it locally. The storage locations may be private to the app (e.g. its internal storage) or be public and therefore accessible by the user or other co-installed apps (e.g. public folders such as Downloads). This control ensures that any sensitive data that is intentionally stored by the app is properly protected independently of the target location.</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>アプリはユーザー、バックエンド、システムサービス、デバイス上の他のアプリなどの多くのソースからの機密データを扱い、通常はローカルに保存する必要があります。保存場所はアプリにとってプライベート (内部ストレージなど) の場合もあれば、パブリック (ダウンロードなどのパブリックフォルダなど) であるためユーザーや他の一緒にインストールされたアプリからアクセス可能な場合もあります。このコントロールによりアプリが意図的に保存する機密データはターゲットの場所とは関係なく適切に保護されます。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Avenir"/>
+      </rPr>
+      <t xml:space="preserve">
+Apps handle sensitive data coming from many sources such as the user, the backend, system services or other apps on the device and usually need to store it locally. The storage locations may be private to the app (e.g. its internal storage) or be public and therefore accessible by the user or other co-installed apps (e.g. public folders such as Downloads). This control ensures that any sensitive data that is intentionally stored by the app is properly protected independently of the target location.</t>
+    </r>
+    <rPh sb="29" eb="30">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>キミツ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>アツカ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>ツウジョウ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="77" eb="81">
+      <t>ホゾンバショ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="109" eb="111">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="155" eb="156">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="157" eb="159">
+      <t>イッショ</t>
+    </rPh>
+    <rPh sb="178" eb="180">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="181" eb="183">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="204" eb="207">
+      <t>イトテキ</t>
+    </rPh>
+    <rPh sb="208" eb="210">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="212" eb="214">
+      <t>キミツ</t>
+    </rPh>
+    <rPh sb="224" eb="226">
+      <t>バショ</t>
+    </rPh>
+    <rPh sb="228" eb="230">
+      <t>カンケイ</t>
+    </rPh>
+    <rPh sb="232" eb="234">
+      <t>テキセツ</t>
+    </rPh>
+    <rPh sb="235" eb="237">
+      <t>ホゴ</t>
+    </rPh>
+    <phoneticPr fontId="32"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>特定の</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Avenir"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>や、バックアップやログなどのシステム機能を使用する副作用として、機密データが意図せずに保存されたり、一般的にアクセスできる場所に公開されることがあります。このコントロールはこのような意図しない漏洩をカバーし、開発者は実際にそれを防ぐ方法を持っています。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Avenir"/>
+      </rPr>
+      <t xml:space="preserve">
+There are cases when sensitive data is unintentionally stored or exposed to publicly accessible locations; typically as a side-effect of using certain APIs, system capabilities such as backups or logs. This control covers this kind of unintentional leaks where the developer actually has a way to prevent it.</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>トクテイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t>フクサヨウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>キミツ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>イト</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="58" eb="61">
+      <t>イッパンテキ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>バショ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>コウカイ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>イト</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ロウエイ</t>
+    </rPh>
     <phoneticPr fontId="32"/>
   </si>
 </sst>
@@ -2166,30 +2324,30 @@
         <v>5</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>130</v>
+      <c r="E4" s="40" t="s">
+        <v>129</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="105">
+    <row r="5" spans="1:7" ht="192.6">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>7</v>
+      <c r="E5" s="40" t="s">
+        <v>130</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -10693,7 +10851,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="2"/>
@@ -10729,16 +10887,16 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="G4" s="12"/>
     </row>
@@ -10746,16 +10904,16 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>15</v>
       </c>
       <c r="G5" s="12"/>
     </row>
@@ -19259,7 +19417,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="2"/>
@@ -19295,16 +19453,16 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="G4" s="12"/>
     </row>
@@ -19312,16 +19470,16 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="12"/>
     </row>
@@ -19329,16 +19487,16 @@
       <c r="A6" s="6"/>
       <c r="B6" s="13"/>
       <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="12"/>
     </row>
@@ -27833,7 +27991,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="2"/>
@@ -27869,16 +28027,16 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="11"/>
     </row>
@@ -27886,16 +28044,16 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -36399,7 +36557,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="2"/>
@@ -36435,16 +36593,16 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="G4" s="8"/>
     </row>
@@ -36452,16 +36610,16 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -36469,16 +36627,16 @@
       <c r="A6" s="6"/>
       <c r="B6" s="13"/>
       <c r="C6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -44973,7 +45131,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="2"/>
@@ -45009,13 +45167,13 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="8"/>
@@ -45024,16 +45182,16 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -45041,16 +45199,16 @@
       <c r="A6" s="6"/>
       <c r="B6" s="13"/>
       <c r="C6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -45058,16 +45216,16 @@
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
       <c r="C7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -53553,7 +53711,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="2"/>
@@ -53588,16 +53746,16 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G4" s="26"/>
     </row>
@@ -53605,16 +53763,16 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G5" s="26"/>
     </row>
@@ -53622,16 +53780,16 @@
       <c r="A6" s="6"/>
       <c r="B6" s="13"/>
       <c r="C6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="G6" s="26"/>
     </row>
@@ -53639,16 +53797,16 @@
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
       <c r="C7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="G7" s="26"/>
     </row>
@@ -62129,7 +62287,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
       <c r="E1" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -62146,10 +62304,10 @@
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
       <c r="D3" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -62166,10 +62324,10 @@
       <c r="B5" s="18"/>
       <c r="C5" s="19"/>
       <c r="D5" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" s="29"/>
     </row>
@@ -62186,10 +62344,10 @@
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
       <c r="D7" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="32"/>
     </row>
@@ -62198,10 +62356,10 @@
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="32"/>
     </row>
@@ -62210,10 +62368,10 @@
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
       <c r="D9" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="32"/>
     </row>
@@ -62222,10 +62380,10 @@
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
       <c r="D10" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="32"/>
     </row>
@@ -62234,10 +62392,10 @@
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="32"/>
     </row>
@@ -62246,10 +62404,10 @@
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
       <c r="D12" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="32"/>
     </row>
@@ -62258,10 +62416,10 @@
       <c r="B13" s="24"/>
       <c r="C13" s="19"/>
       <c r="D13" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="32"/>
     </row>
@@ -62278,10 +62436,10 @@
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" s="29"/>
     </row>
@@ -62298,10 +62456,10 @@
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -62310,10 +62468,10 @@
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F18" s="32"/>
     </row>
@@ -62322,10 +62480,10 @@
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="32"/>
     </row>
@@ -62334,10 +62492,10 @@
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
       <c r="D20" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="32"/>
     </row>
@@ -62346,10 +62504,10 @@
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
       <c r="D21" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" s="32"/>
     </row>
@@ -62358,10 +62516,10 @@
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
       <c r="D22" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="32"/>
     </row>
@@ -62370,10 +62528,10 @@
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
       <c r="D23" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="32"/>
     </row>
@@ -62382,10 +62540,10 @@
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="D24" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F24" s="32"/>
     </row>
@@ -62402,7 +62560,7 @@
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
@@ -62420,7 +62578,7 @@
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" s="46"/>
       <c r="F28" s="46"/>
@@ -62438,7 +62596,7 @@
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
       <c r="D30" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="32"/>
@@ -62456,7 +62614,7 @@
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
       <c r="D32" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="46"/>
       <c r="F32" s="46"/>
@@ -62493,7 +62651,7 @@
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
       <c r="D36" s="45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E36" s="46"/>
       <c r="F36" s="46"/>
@@ -62511,7 +62669,7 @@
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
       <c r="D38" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" s="46"/>
       <c r="F38" s="32"/>
@@ -62529,7 +62687,7 @@
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
       <c r="D40" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E40" s="46"/>
       <c r="F40" s="46"/>
@@ -62547,7 +62705,7 @@
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
       <c r="D42" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42" s="46"/>
       <c r="F42" s="46"/>
@@ -62584,7 +62742,7 @@
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
       <c r="D46" s="48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
@@ -62602,7 +62760,7 @@
       <c r="B48" s="18"/>
       <c r="C48" s="19"/>
       <c r="D48" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
@@ -62620,7 +62778,7 @@
       <c r="B50" s="18"/>
       <c r="C50" s="19"/>
       <c r="D50" s="47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="32"/>

</xml_diff>